<commit_message>
Next update and test
Added bundle profile and updated the messagedefinition profile
</commit_message>
<xml_diff>
--- a/output/PAO-messagedefinition4.xlsx
+++ b/output/PAO-messagedefinition4.xlsx
@@ -2519,7 +2519,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" hidden="true">
+    <row r="13">
       <c r="A13" t="s" s="2">
         <v>121</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>50</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="H13" t="s" s="2">
         <v>41</v>
@@ -2633,7 +2633,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" hidden="true">
+    <row r="14">
       <c r="A14" t="s" s="2">
         <v>127</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>50</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="H14" t="s" s="2">
         <v>41</v>
@@ -2749,7 +2749,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" hidden="true">
+    <row r="15">
       <c r="A15" t="s" s="2">
         <v>133</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>50</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="H15" t="s" s="2">
         <v>41</v>
@@ -2975,7 +2975,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" hidden="true">
+    <row r="17">
       <c r="A17" t="s" s="2">
         <v>142</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>50</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="H17" t="s" s="2">
         <v>51</v>

</xml_diff>

<commit_message>
Includes all initial profiles
</commit_message>
<xml_diff>
--- a/output/PAO-messagedefinition4.xlsx
+++ b/output/PAO-messagedefinition4.xlsx
@@ -4347,7 +4347,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" hidden="true">
+    <row r="29">
       <c r="A29" t="s" s="2">
         <v>221</v>
       </c>
@@ -4363,7 +4363,7 @@
         <v>50</v>
       </c>
       <c r="G29" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="H29" t="s" s="2">
         <v>41</v>
@@ -4459,7 +4459,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" hidden="true">
+    <row r="30">
       <c r="A30" t="s" s="2">
         <v>228</v>
       </c>
@@ -4469,13 +4469,13 @@
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="F30" t="s" s="2">
         <v>50</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="H30" t="s" s="2">
         <v>41</v>
@@ -4571,7 +4571,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" hidden="true">
+    <row r="31">
       <c r="A31" t="s" s="2">
         <v>233</v>
       </c>
@@ -4581,13 +4581,13 @@
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="F31" t="s" s="2">
         <v>43</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="H31" t="s" s="2">
         <v>41</v>
@@ -5025,7 +5025,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" hidden="true">
+    <row r="35">
       <c r="A35" t="s" s="2">
         <v>251</v>
       </c>
@@ -5041,7 +5041,7 @@
         <v>50</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="H35" t="s" s="2">
         <v>41</v>
@@ -5139,7 +5139,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" hidden="true">
+    <row r="36">
       <c r="A36" t="s" s="2">
         <v>257</v>
       </c>
@@ -5155,7 +5155,7 @@
         <v>50</v>
       </c>
       <c r="G36" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="H36" t="s" s="2">
         <v>41</v>

</xml_diff>